<commit_message>
Updated selected sample pdf lists
</commit_message>
<xml_diff>
--- a/SelectedSamplesPaper.xlsx
+++ b/SelectedSamplesPaper.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13410"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610"/>
   </bookViews>
   <sheets>
-    <sheet name="Selected_Original" sheetId="1" r:id="rId1"/>
+    <sheet name="Selected_Final" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="83">
   <si>
     <t>CLAY_Norm</t>
   </si>
@@ -231,9 +231,6 @@
   </si>
   <si>
     <t>2017-105</t>
-  </si>
-  <si>
-    <t>2011-112</t>
   </si>
   <si>
     <t>2011-106</t>
@@ -655,22 +652,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J123"/>
+  <dimension ref="A1:J121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="O42" sqref="O42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="12" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="6" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="5" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="5.28515625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.7109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="7.7109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.7109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.28515625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -2243,25 +2240,25 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
-        <v>29.37062937062937</v>
+        <v>11.553784860557768</v>
       </c>
       <c r="B50" s="2">
-        <v>41.658341658341662</v>
+        <v>50.398406374501988</v>
       </c>
       <c r="C50" s="2">
-        <v>28.971028971028971</v>
+        <v>38.047808764940235</v>
       </c>
       <c r="D50" s="2">
-        <v>29</v>
+        <v>38.200000000000003</v>
       </c>
       <c r="E50" s="2">
-        <v>41.7</v>
+        <v>50.6</v>
       </c>
       <c r="F50" s="2">
-        <v>29.4</v>
+        <v>11.6</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>69</v>
+        <v>10</v>
       </c>
       <c r="H50" s="3" t="s">
         <v>11</v>
@@ -2270,30 +2267,30 @@
         <v>12</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
-        <v>11.553784860557768</v>
+        <v>6.1220413462498753</v>
       </c>
       <c r="B51" s="2">
-        <v>50.398406374501988</v>
+        <v>17.477279536602417</v>
       </c>
       <c r="C51" s="2">
-        <v>38.047808764940235</v>
+        <v>76.400679117147718</v>
       </c>
       <c r="D51" s="2">
-        <v>38.200000000000003</v>
+        <v>76.5</v>
       </c>
       <c r="E51" s="2">
-        <v>50.6</v>
+        <v>17.5</v>
       </c>
       <c r="F51" s="2">
-        <v>11.6</v>
+        <v>6.13</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="H51" s="3" t="s">
         <v>11</v>
@@ -2302,30 +2299,30 @@
         <v>12</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
-        <v>6.1220413462498753</v>
+        <v>4.9751243781094532</v>
       </c>
       <c r="B52" s="2">
-        <v>17.477279536602417</v>
+        <v>21.890547263681594</v>
       </c>
       <c r="C52" s="2">
-        <v>76.400679117147718</v>
+        <v>73.134328358208961</v>
       </c>
       <c r="D52" s="2">
-        <v>76.5</v>
+        <v>73.5</v>
       </c>
       <c r="E52" s="2">
-        <v>17.5</v>
+        <v>22</v>
       </c>
       <c r="F52" s="2">
-        <v>6.13</v>
+        <v>5</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H52" s="3" t="s">
         <v>11</v>
@@ -2334,30 +2331,30 @@
         <v>12</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
-        <v>4.9751243781094532</v>
+        <v>10.030090270812437</v>
       </c>
       <c r="B53" s="2">
-        <v>21.890547263681594</v>
+        <v>33.801404212637919</v>
       </c>
       <c r="C53" s="2">
-        <v>73.134328358208961</v>
+        <v>56.168505516549651</v>
       </c>
       <c r="D53" s="2">
-        <v>73.5</v>
+        <v>56</v>
       </c>
       <c r="E53" s="2">
-        <v>22</v>
+        <v>33.700000000000003</v>
       </c>
       <c r="F53" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H53" s="3" t="s">
         <v>11</v>
@@ -2371,25 +2368,25 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <v>10.030090270812437</v>
+        <v>17.119838872104733</v>
       </c>
       <c r="B54" s="2">
-        <v>33.801404212637919</v>
+        <v>38.670694864048336</v>
       </c>
       <c r="C54" s="2">
-        <v>56.168505516549651</v>
+        <v>44.209466263846927</v>
       </c>
       <c r="D54" s="2">
-        <v>56</v>
+        <v>43.9</v>
       </c>
       <c r="E54" s="2">
-        <v>33.700000000000003</v>
+        <v>38.4</v>
       </c>
       <c r="F54" s="2">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H54" s="3" t="s">
         <v>11</v>
@@ -2398,30 +2395,30 @@
         <v>12</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
-        <v>17.119838872104733</v>
+        <v>51.832993890020362</v>
       </c>
       <c r="B55" s="2">
-        <v>38.670694864048336</v>
+        <v>29.837067209775967</v>
       </c>
       <c r="C55" s="2">
-        <v>44.209466263846927</v>
+        <v>18.329938900203665</v>
       </c>
       <c r="D55" s="2">
-        <v>43.9</v>
+        <v>18</v>
       </c>
       <c r="E55" s="2">
-        <v>38.4</v>
+        <v>29.3</v>
       </c>
       <c r="F55" s="2">
-        <v>17</v>
+        <v>50.9</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="H55" s="3" t="s">
         <v>11</v>
@@ -2430,27 +2427,27 @@
         <v>12</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
-        <v>51.832993890020362</v>
+        <v>21.449851042701091</v>
       </c>
       <c r="B56" s="2">
-        <v>29.837067209775967</v>
+        <v>15.392254220456801</v>
       </c>
       <c r="C56" s="2">
-        <v>18.329938900203665</v>
+        <v>63.157894736842103</v>
       </c>
       <c r="D56" s="2">
-        <v>18</v>
+        <v>63.6</v>
       </c>
       <c r="E56" s="2">
-        <v>29.3</v>
+        <v>15.5</v>
       </c>
       <c r="F56" s="2">
-        <v>50.9</v>
+        <v>21.6</v>
       </c>
       <c r="G56" s="3" t="s">
         <v>70</v>
@@ -2462,27 +2459,27 @@
         <v>12</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
-        <v>21.449851042701091</v>
+        <v>2.0202020202020203</v>
       </c>
       <c r="B57" s="2">
-        <v>15.392254220456801</v>
+        <v>3.0303030303030303</v>
       </c>
       <c r="C57" s="2">
-        <v>63.157894736842103</v>
+        <v>94.949494949494962</v>
       </c>
       <c r="D57" s="2">
-        <v>63.6</v>
+        <v>94</v>
       </c>
       <c r="E57" s="2">
-        <v>15.5</v>
+        <v>3</v>
       </c>
       <c r="F57" s="2">
-        <v>21.6</v>
+        <v>2</v>
       </c>
       <c r="G57" s="3" t="s">
         <v>71</v>
@@ -2494,27 +2491,27 @@
         <v>12</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
-        <v>2.0202020202020203</v>
+        <v>26.043737574552683</v>
       </c>
       <c r="B58" s="2">
-        <v>3.0303030303030303</v>
+        <v>19.284294234592444</v>
       </c>
       <c r="C58" s="2">
-        <v>94.949494949494962</v>
+        <v>54.671968190854869</v>
       </c>
       <c r="D58" s="2">
-        <v>94</v>
+        <v>55</v>
       </c>
       <c r="E58" s="2">
-        <v>3</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="F58" s="2">
-        <v>2</v>
+        <v>26.2</v>
       </c>
       <c r="G58" s="3" t="s">
         <v>72</v>
@@ -2526,27 +2523,27 @@
         <v>12</v>
       </c>
       <c r="J58" s="3" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
-        <v>26.043737574552683</v>
+        <v>1.9980019980019978</v>
       </c>
       <c r="B59" s="2">
-        <v>19.284294234592444</v>
+        <v>2.197802197802198</v>
       </c>
       <c r="C59" s="2">
-        <v>54.671968190854869</v>
+        <v>95.8041958041958</v>
       </c>
       <c r="D59" s="2">
-        <v>55</v>
+        <v>95.9</v>
       </c>
       <c r="E59" s="2">
-        <v>19.399999999999999</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F59" s="2">
-        <v>26.2</v>
+        <v>2</v>
       </c>
       <c r="G59" s="3" t="s">
         <v>73</v>
@@ -2558,27 +2555,27 @@
         <v>12</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
-        <v>1.9980019980019978</v>
+        <v>20.48929663608563</v>
       </c>
       <c r="B60" s="2">
-        <v>2.197802197802198</v>
+        <v>15.290519877675843</v>
       </c>
       <c r="C60" s="2">
-        <v>95.8041958041958</v>
+        <v>64.22018348623854</v>
       </c>
       <c r="D60" s="2">
-        <v>95.9</v>
+        <v>63</v>
       </c>
       <c r="E60" s="2">
-        <v>2.2000000000000002</v>
+        <v>15</v>
       </c>
       <c r="F60" s="2">
-        <v>2</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="G60" s="3" t="s">
         <v>74</v>
@@ -2590,27 +2587,27 @@
         <v>12</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
-        <v>20.48929663608563</v>
+        <v>55.034895314057827</v>
       </c>
       <c r="B61" s="2">
-        <v>15.290519877675843</v>
+        <v>28.51445663010967</v>
       </c>
       <c r="C61" s="2">
-        <v>64.22018348623854</v>
+        <v>16.450648055832502</v>
       </c>
       <c r="D61" s="2">
-        <v>63</v>
+        <v>16.5</v>
       </c>
       <c r="E61" s="2">
-        <v>15</v>
+        <v>28.6</v>
       </c>
       <c r="F61" s="2">
-        <v>20.100000000000001</v>
+        <v>55.2</v>
       </c>
       <c r="G61" s="3" t="s">
         <v>75</v>
@@ -2622,27 +2619,27 @@
         <v>12</v>
       </c>
       <c r="J61" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
-        <v>55.034895314057827</v>
+        <v>29.012961116650054</v>
       </c>
       <c r="B62" s="2">
-        <v>28.51445663010967</v>
+        <v>24.127617148554336</v>
       </c>
       <c r="C62" s="2">
-        <v>16.450648055832502</v>
+        <v>46.859421734795617</v>
       </c>
       <c r="D62" s="2">
-        <v>16.5</v>
+        <v>47</v>
       </c>
       <c r="E62" s="2">
-        <v>28.6</v>
+        <v>24.2</v>
       </c>
       <c r="F62" s="2">
-        <v>55.2</v>
+        <v>29.1</v>
       </c>
       <c r="G62" s="3" t="s">
         <v>76</v>
@@ -2654,27 +2651,27 @@
         <v>12</v>
       </c>
       <c r="J62" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
-        <v>29.012961116650054</v>
+        <v>31.542968749999996</v>
       </c>
       <c r="B63" s="2">
-        <v>24.127617148554336</v>
+        <v>20.60546875</v>
       </c>
       <c r="C63" s="2">
-        <v>46.859421734795617</v>
+        <v>47.8515625</v>
       </c>
       <c r="D63" s="2">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E63" s="2">
-        <v>24.2</v>
+        <v>21.1</v>
       </c>
       <c r="F63" s="2">
-        <v>29.1</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="G63" s="3" t="s">
         <v>77</v>
@@ -2691,22 +2688,22 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
-        <v>31.542968749999996</v>
+        <v>54.294478527607367</v>
       </c>
       <c r="B64" s="2">
-        <v>20.60546875</v>
+        <v>38.854805725971374</v>
       </c>
       <c r="C64" s="2">
-        <v>47.8515625</v>
+        <v>6.850715746421268</v>
       </c>
       <c r="D64" s="2">
-        <v>49</v>
+        <v>6.7</v>
       </c>
       <c r="E64" s="2">
-        <v>21.1</v>
+        <v>38</v>
       </c>
       <c r="F64" s="2">
-        <v>32.299999999999997</v>
+        <v>53.1</v>
       </c>
       <c r="G64" s="3" t="s">
         <v>78</v>
@@ -2718,100 +2715,100 @@
         <v>12</v>
       </c>
       <c r="J64" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
-        <v>54.294478527607367</v>
+        <v>8.6629944917376047</v>
       </c>
       <c r="B65" s="2">
-        <v>38.854805725971374</v>
+        <v>54.28142213319979</v>
       </c>
       <c r="C65" s="2">
-        <v>6.850715746421268</v>
+        <v>37.055583375062589</v>
       </c>
       <c r="D65" s="2">
-        <v>6.7</v>
+        <v>37</v>
       </c>
       <c r="E65" s="2">
-        <v>38</v>
+        <v>54.2</v>
       </c>
       <c r="F65" s="2">
-        <v>53.1</v>
+        <v>8.65</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="H65" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="J65" s="3" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
-        <v>8.6629944917376047</v>
+        <v>5.5226824457593677</v>
       </c>
       <c r="B66" s="2">
-        <v>54.28142213319979</v>
+        <v>12.721893491124259</v>
       </c>
       <c r="C66" s="2">
-        <v>37.055583375062589</v>
+        <v>81.755424063116365</v>
       </c>
       <c r="D66" s="2">
-        <v>37</v>
+        <v>82.9</v>
       </c>
       <c r="E66" s="2">
-        <v>54.2</v>
+        <v>12.9</v>
       </c>
       <c r="F66" s="2">
-        <v>8.65</v>
+        <v>5.6</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="H66" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J66" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
-        <v>5.5226824457593677</v>
+        <v>4.2095790420957906</v>
       </c>
       <c r="B67" s="2">
-        <v>12.721893491124259</v>
+        <v>17.498250174982502</v>
       </c>
       <c r="C67" s="2">
-        <v>81.755424063116365</v>
+        <v>78.292170782921715</v>
       </c>
       <c r="D67" s="2">
-        <v>82.9</v>
+        <v>78.3</v>
       </c>
       <c r="E67" s="2">
-        <v>12.9</v>
+        <v>17.5</v>
       </c>
       <c r="F67" s="2">
-        <v>5.6</v>
+        <v>4.21</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H67" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J67" s="3" t="s">
         <v>15</v>
@@ -2819,255 +2816,255 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
-        <v>4.2095790420957906</v>
+        <v>11.84738955823293</v>
       </c>
       <c r="B68" s="2">
-        <v>17.498250174982502</v>
+        <v>33.232931726907623</v>
       </c>
       <c r="C68" s="2">
-        <v>78.292170782921715</v>
+        <v>54.91967871485943</v>
       </c>
       <c r="D68" s="2">
-        <v>78.3</v>
+        <v>54.7</v>
       </c>
       <c r="E68" s="2">
-        <v>17.5</v>
+        <v>33.1</v>
       </c>
       <c r="F68" s="2">
-        <v>4.21</v>
+        <v>11.8</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H68" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J68" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
-        <v>11.84738955823293</v>
+        <v>16.701030927835049</v>
       </c>
       <c r="B69" s="2">
-        <v>33.232931726907623</v>
+        <v>31.649484536082468</v>
       </c>
       <c r="C69" s="2">
-        <v>54.91967871485943</v>
+        <v>51.649484536082468</v>
       </c>
       <c r="D69" s="2">
-        <v>54.7</v>
+        <v>50.1</v>
       </c>
       <c r="E69" s="2">
-        <v>33.1</v>
+        <v>30.7</v>
       </c>
       <c r="F69" s="2">
-        <v>11.8</v>
+        <v>16.2</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H69" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I69" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J69" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
-        <v>16.701030927835049</v>
+        <v>17.8</v>
       </c>
       <c r="B70" s="2">
-        <v>31.649484536082468</v>
+        <v>29.2</v>
       </c>
       <c r="C70" s="2">
-        <v>51.649484536082468</v>
+        <v>53</v>
       </c>
       <c r="D70" s="2">
-        <v>50.1</v>
+        <v>53</v>
       </c>
       <c r="E70" s="2">
-        <v>30.7</v>
+        <v>29.2</v>
       </c>
       <c r="F70" s="2">
-        <v>16.2</v>
+        <v>17.8</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H70" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I70" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J70" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
-        <v>17.8</v>
+        <v>26</v>
       </c>
       <c r="B71" s="2">
-        <v>29.2</v>
+        <v>64</v>
       </c>
       <c r="C71" s="2">
-        <v>53</v>
+        <v>10</v>
       </c>
       <c r="D71" s="2">
-        <v>53</v>
+        <v>10</v>
       </c>
       <c r="E71" s="2">
-        <v>29.2</v>
+        <v>64</v>
       </c>
       <c r="F71" s="2">
-        <v>17.8</v>
+        <v>26</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H71" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I71" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J71" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
-        <v>26</v>
+        <v>10.159362549800795</v>
       </c>
       <c r="B72" s="2">
-        <v>64</v>
+        <v>27.888446215139439</v>
       </c>
       <c r="C72" s="2">
-        <v>10</v>
+        <v>61.952191235059757</v>
       </c>
       <c r="D72" s="2">
-        <v>10</v>
+        <v>62.2</v>
       </c>
       <c r="E72" s="2">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="F72" s="2">
-        <v>26</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H72" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I72" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J72" s="3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
-        <v>10.159362549800795</v>
+        <v>9.9800399201596797</v>
       </c>
       <c r="B73" s="2">
-        <v>27.888446215139439</v>
+        <v>7.1856287425149699</v>
       </c>
       <c r="C73" s="2">
-        <v>61.952191235059757</v>
+        <v>82.834331337325338</v>
       </c>
       <c r="D73" s="2">
-        <v>62.2</v>
+        <v>83</v>
       </c>
       <c r="E73" s="2">
-        <v>28</v>
+        <v>7.2</v>
       </c>
       <c r="F73" s="2">
-        <v>10.199999999999999</v>
+        <v>10</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H73" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I73" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J73" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
-        <v>9.9800399201596797</v>
+        <v>16.032064128256515</v>
       </c>
       <c r="B74" s="2">
-        <v>7.1856287425149699</v>
+        <v>68.136272545090193</v>
       </c>
       <c r="C74" s="2">
-        <v>82.834331337325338</v>
+        <v>15.83166332665331</v>
       </c>
       <c r="D74" s="2">
-        <v>83</v>
+        <v>15.8</v>
       </c>
       <c r="E74" s="2">
-        <v>7.2</v>
+        <v>68</v>
       </c>
       <c r="F74" s="2">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H74" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I74" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J74" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
-        <v>16.032064128256515</v>
+        <v>15.2</v>
       </c>
       <c r="B75" s="2">
-        <v>68.136272545090193</v>
+        <v>69.8</v>
       </c>
       <c r="C75" s="2">
-        <v>15.83166332665331</v>
+        <v>15</v>
       </c>
       <c r="D75" s="2">
-        <v>15.8</v>
+        <v>15</v>
       </c>
       <c r="E75" s="2">
-        <v>68</v>
+        <v>69.8</v>
       </c>
       <c r="F75" s="2">
-        <v>16</v>
+        <v>15.2</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H75" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I75" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J75" s="3" t="s">
         <v>13</v>
@@ -3075,255 +3072,255 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
-        <v>15.2</v>
+        <v>8.2733812949640289</v>
       </c>
       <c r="B76" s="2">
-        <v>69.8</v>
+        <v>17.985611510791369</v>
       </c>
       <c r="C76" s="2">
-        <v>15</v>
+        <v>73.741007194244602</v>
       </c>
       <c r="D76" s="2">
-        <v>15</v>
+        <v>73.8</v>
       </c>
       <c r="E76" s="2">
-        <v>69.8</v>
+        <v>18</v>
       </c>
       <c r="F76" s="2">
-        <v>15.2</v>
+        <v>8.2799999999999994</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H76" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I76" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J76" s="3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
-        <v>8.2733812949640289</v>
+        <v>19.807923169267706</v>
       </c>
       <c r="B77" s="2">
-        <v>17.985611510791369</v>
+        <v>72.028811524609836</v>
       </c>
       <c r="C77" s="2">
-        <v>73.741007194244602</v>
+        <v>8.1632653061224492</v>
       </c>
       <c r="D77" s="2">
-        <v>73.8</v>
+        <v>8.16</v>
       </c>
       <c r="E77" s="2">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="F77" s="2">
-        <v>8.2799999999999994</v>
+        <v>19.8</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H77" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I77" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J77" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
-        <v>19.807923169267706</v>
+        <v>3.3930537483735361</v>
       </c>
       <c r="B78" s="2">
-        <v>72.028811524609836</v>
+        <v>7.3265939345410871</v>
       </c>
       <c r="C78" s="2">
-        <v>8.1632653061224492</v>
+        <v>89.280352317085374</v>
       </c>
       <c r="D78" s="2">
-        <v>8.16</v>
+        <v>89.2</v>
       </c>
       <c r="E78" s="2">
-        <v>72</v>
+        <v>7.32</v>
       </c>
       <c r="F78" s="2">
-        <v>19.8</v>
+        <v>3.39</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H78" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I78" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J78" s="3" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
-        <v>3.3930537483735361</v>
+        <v>13.340020060180542</v>
       </c>
       <c r="B79" s="2">
-        <v>7.3265939345410871</v>
+        <v>64.694082246740223</v>
       </c>
       <c r="C79" s="2">
-        <v>89.280352317085374</v>
+        <v>21.965897693079235</v>
       </c>
       <c r="D79" s="2">
-        <v>89.2</v>
+        <v>21.9</v>
       </c>
       <c r="E79" s="2">
-        <v>7.32</v>
+        <v>64.5</v>
       </c>
       <c r="F79" s="2">
-        <v>3.39</v>
+        <v>13.3</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H79" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I79" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J79" s="3" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
-        <v>13.340020060180542</v>
+        <v>22.554890219560878</v>
       </c>
       <c r="B80" s="2">
-        <v>64.694082246740223</v>
+        <v>34.830339321357279</v>
       </c>
       <c r="C80" s="2">
-        <v>21.965897693079235</v>
+        <v>42.614770459081839</v>
       </c>
       <c r="D80" s="2">
-        <v>21.9</v>
+        <v>42.7</v>
       </c>
       <c r="E80" s="2">
-        <v>64.5</v>
+        <v>34.9</v>
       </c>
       <c r="F80" s="2">
-        <v>13.3</v>
+        <v>22.6</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H80" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I80" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J80" s="3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
-        <v>22.554890219560878</v>
+        <v>27.678571428571427</v>
       </c>
       <c r="B81" s="2">
-        <v>34.830339321357279</v>
+        <v>38.789682539682545</v>
       </c>
       <c r="C81" s="2">
-        <v>42.614770459081839</v>
+        <v>33.531746031746032</v>
       </c>
       <c r="D81" s="2">
-        <v>42.7</v>
+        <v>33.799999999999997</v>
       </c>
       <c r="E81" s="2">
-        <v>34.9</v>
+        <v>39.1</v>
       </c>
       <c r="F81" s="2">
-        <v>22.6</v>
+        <v>27.9</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H81" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I81" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J81" s="3" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
-        <v>27.678571428571427</v>
+        <v>3.6892621475704859</v>
       </c>
       <c r="B82" s="2">
-        <v>38.789682539682545</v>
+        <v>8.0283943211357727</v>
       </c>
       <c r="C82" s="2">
-        <v>33.531746031746032</v>
+        <v>88.282343531293733</v>
       </c>
       <c r="D82" s="2">
-        <v>33.799999999999997</v>
+        <v>88.3</v>
       </c>
       <c r="E82" s="2">
-        <v>39.1</v>
+        <v>8.0299999999999994</v>
       </c>
       <c r="F82" s="2">
-        <v>27.9</v>
+        <v>3.69</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H82" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I82" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J82" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
-        <v>3.6892621475704859</v>
+        <v>2.0233230339878401</v>
       </c>
       <c r="B83" s="2">
-        <v>8.0283943211357727</v>
+        <v>1.5947373666899234</v>
       </c>
       <c r="C83" s="2">
-        <v>88.282343531293733</v>
+        <v>96.381939599322251</v>
       </c>
       <c r="D83" s="2">
-        <v>88.3</v>
+        <v>96.7</v>
       </c>
       <c r="E83" s="2">
-        <v>8.0299999999999994</v>
+        <v>1.6</v>
       </c>
       <c r="F83" s="2">
-        <v>3.69</v>
+        <v>2.0299999999999998</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H83" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I83" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J83" s="3" t="s">
         <v>30</v>
@@ -3331,31 +3328,31 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
-        <v>2.0233230339878401</v>
+        <v>2.5</v>
       </c>
       <c r="B84" s="2">
-        <v>1.5947373666899234</v>
+        <v>10.3</v>
       </c>
       <c r="C84" s="2">
-        <v>96.381939599322251</v>
+        <v>87.2</v>
       </c>
       <c r="D84" s="2">
-        <v>96.7</v>
+        <v>87.2</v>
       </c>
       <c r="E84" s="2">
-        <v>1.6</v>
+        <v>10.3</v>
       </c>
       <c r="F84" s="2">
-        <v>2.0299999999999998</v>
+        <v>2.5</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H84" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I84" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J84" s="3" t="s">
         <v>30</v>
@@ -3363,63 +3360,63 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
-        <v>2.5</v>
+        <v>16.666666666666664</v>
       </c>
       <c r="B85" s="2">
-        <v>10.3</v>
+        <v>34.131736526946106</v>
       </c>
       <c r="C85" s="2">
-        <v>87.2</v>
+        <v>49.201596806387222</v>
       </c>
       <c r="D85" s="2">
-        <v>87.2</v>
+        <v>49.3</v>
       </c>
       <c r="E85" s="2">
-        <v>10.3</v>
+        <v>34.200000000000003</v>
       </c>
       <c r="F85" s="2">
-        <v>2.5</v>
+        <v>16.7</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H85" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I85" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J85" s="3" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
-        <v>16.666666666666664</v>
+        <v>18.946301925025331</v>
       </c>
       <c r="B86" s="2">
-        <v>34.131736526946106</v>
+        <v>36.372847011144884</v>
       </c>
       <c r="C86" s="2">
-        <v>49.201596806387222</v>
+        <v>44.680851063829792</v>
       </c>
       <c r="D86" s="2">
-        <v>49.3</v>
+        <v>44.1</v>
       </c>
       <c r="E86" s="2">
-        <v>34.200000000000003</v>
+        <v>35.9</v>
       </c>
       <c r="F86" s="2">
-        <v>16.7</v>
+        <v>18.7</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H86" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I86" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J86" s="3" t="s">
         <v>20</v>
@@ -3427,127 +3424,127 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
-        <v>18.946301925025331</v>
+        <v>21.479229989868287</v>
       </c>
       <c r="B87" s="2">
-        <v>36.372847011144884</v>
+        <v>10.131712259371835</v>
       </c>
       <c r="C87" s="2">
-        <v>44.680851063829792</v>
+        <v>68.389057750759889</v>
       </c>
       <c r="D87" s="2">
-        <v>44.1</v>
+        <v>67.5</v>
       </c>
       <c r="E87" s="2">
-        <v>35.9</v>
+        <v>10</v>
       </c>
       <c r="F87" s="2">
-        <v>18.7</v>
+        <v>21.2</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H87" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I87" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J87" s="3" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
-        <v>21.479229989868287</v>
+        <v>50.2</v>
       </c>
       <c r="B88" s="2">
-        <v>10.131712259371835</v>
+        <v>37.299999999999997</v>
       </c>
       <c r="C88" s="2">
-        <v>68.389057750759889</v>
+        <v>12.5</v>
       </c>
       <c r="D88" s="2">
-        <v>67.5</v>
+        <v>12.5</v>
       </c>
       <c r="E88" s="2">
-        <v>10</v>
+        <v>37.299999999999997</v>
       </c>
       <c r="F88" s="2">
-        <v>21.2</v>
+        <v>50.2</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H88" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I88" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J88" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
-        <v>50.2</v>
+        <v>12.024048096192384</v>
       </c>
       <c r="B89" s="2">
-        <v>37.299999999999997</v>
+        <v>21.943887775551097</v>
       </c>
       <c r="C89" s="2">
-        <v>12.5</v>
+        <v>66.032064128256508</v>
       </c>
       <c r="D89" s="2">
-        <v>12.5</v>
+        <v>65.900000000000006</v>
       </c>
       <c r="E89" s="2">
-        <v>37.299999999999997</v>
+        <v>21.9</v>
       </c>
       <c r="F89" s="2">
-        <v>50.2</v>
+        <v>12</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H89" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I89" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J89" s="3" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
-        <v>12.024048096192384</v>
+        <v>7.7431633777421629</v>
       </c>
       <c r="B90" s="2">
-        <v>21.943887775551097</v>
+        <v>20.134228187919465</v>
       </c>
       <c r="C90" s="2">
-        <v>66.032064128256508</v>
+        <v>72.122608434338389</v>
       </c>
       <c r="D90" s="2">
-        <v>65.900000000000006</v>
+        <v>72</v>
       </c>
       <c r="E90" s="2">
-        <v>21.9</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="F90" s="2">
-        <v>12</v>
+        <v>7.73</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H90" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I90" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J90" s="3" t="s">
         <v>17</v>
@@ -3555,31 +3552,31 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
-        <v>7.7431633777421629</v>
+        <v>13.39031339031339</v>
       </c>
       <c r="B91" s="2">
-        <v>20.134228187919465</v>
+        <v>32.478632478632484</v>
       </c>
       <c r="C91" s="2">
-        <v>72.122608434338389</v>
+        <v>54.131054131054128</v>
       </c>
       <c r="D91" s="2">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="E91" s="2">
-        <v>20.100000000000001</v>
+        <v>34.200000000000003</v>
       </c>
       <c r="F91" s="2">
-        <v>7.73</v>
+        <v>14.1</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H91" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I91" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J91" s="3" t="s">
         <v>17</v>
@@ -3587,95 +3584,95 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
-        <v>13.39031339031339</v>
+        <v>5.5445544554455441</v>
       </c>
       <c r="B92" s="2">
-        <v>32.478632478632484</v>
+        <v>5.5445544554455441</v>
       </c>
       <c r="C92" s="2">
-        <v>54.131054131054128</v>
+        <v>88.910891089108901</v>
       </c>
       <c r="D92" s="2">
-        <v>57</v>
+        <v>89.8</v>
       </c>
       <c r="E92" s="2">
-        <v>34.200000000000003</v>
+        <v>5.6</v>
       </c>
       <c r="F92" s="2">
-        <v>14.1</v>
+        <v>5.6</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H92" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I92" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J92" s="3" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
-        <v>5.5445544554455441</v>
+        <v>47.821878025169411</v>
       </c>
       <c r="B93" s="2">
-        <v>5.5445544554455441</v>
+        <v>30.977734753146176</v>
       </c>
       <c r="C93" s="2">
-        <v>88.910891089108901</v>
+        <v>21.200387221684412</v>
       </c>
       <c r="D93" s="2">
-        <v>89.8</v>
+        <v>21.9</v>
       </c>
       <c r="E93" s="2">
-        <v>5.6</v>
+        <v>32</v>
       </c>
       <c r="F93" s="2">
-        <v>5.6</v>
+        <v>49.4</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H93" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I93" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J93" s="3" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
-        <v>47.821878025169411</v>
+        <v>49.3</v>
       </c>
       <c r="B94" s="2">
-        <v>30.977734753146176</v>
+        <v>31.8</v>
       </c>
       <c r="C94" s="2">
-        <v>21.200387221684412</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="D94" s="2">
-        <v>21.9</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="E94" s="2">
-        <v>32</v>
+        <v>31.8</v>
       </c>
       <c r="F94" s="2">
-        <v>49.4</v>
+        <v>49.3</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H94" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I94" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J94" s="3" t="s">
         <v>43</v>
@@ -3683,31 +3680,31 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
-        <v>49.3</v>
+        <v>50.821256038647341</v>
       </c>
       <c r="B95" s="2">
-        <v>31.8</v>
+        <v>31.884057971014492</v>
       </c>
       <c r="C95" s="2">
-        <v>18.899999999999999</v>
+        <v>17.294685990338163</v>
       </c>
       <c r="D95" s="2">
-        <v>18.899999999999999</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="E95" s="2">
-        <v>31.8</v>
+        <v>33</v>
       </c>
       <c r="F95" s="2">
-        <v>49.3</v>
+        <v>52.6</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H95" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I95" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J95" s="3" t="s">
         <v>43</v>
@@ -3715,255 +3712,255 @@
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
-        <v>50.821256038647341</v>
+        <v>26.156941649899395</v>
       </c>
       <c r="B96" s="2">
-        <v>31.884057971014492</v>
+        <v>18.410462776659958</v>
       </c>
       <c r="C96" s="2">
-        <v>17.294685990338163</v>
+        <v>55.432595573440643</v>
       </c>
       <c r="D96" s="2">
-        <v>17.899999999999999</v>
+        <v>55.1</v>
       </c>
       <c r="E96" s="2">
-        <v>33</v>
+        <v>18.3</v>
       </c>
       <c r="F96" s="2">
-        <v>52.6</v>
+        <v>26</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H96" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I96" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J96" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
-        <v>26.156941649899395</v>
+        <v>30.694980694980696</v>
       </c>
       <c r="B97" s="2">
-        <v>18.410462776659958</v>
+        <v>55.115830115830121</v>
       </c>
       <c r="C97" s="2">
-        <v>55.432595573440643</v>
+        <v>14.189189189189189</v>
       </c>
       <c r="D97" s="2">
-        <v>55.1</v>
+        <v>14.7</v>
       </c>
       <c r="E97" s="2">
-        <v>18.3</v>
+        <v>57.1</v>
       </c>
       <c r="F97" s="2">
-        <v>26</v>
+        <v>31.8</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H97" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I97" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J97" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
-        <v>30.694980694980696</v>
+        <v>11</v>
       </c>
       <c r="B98" s="2">
-        <v>55.115830115830121</v>
+        <v>7</v>
       </c>
       <c r="C98" s="2">
-        <v>14.189189189189189</v>
+        <v>82</v>
       </c>
       <c r="D98" s="2">
-        <v>14.7</v>
+        <v>82</v>
       </c>
       <c r="E98" s="2">
-        <v>57.1</v>
+        <v>7</v>
       </c>
       <c r="F98" s="2">
-        <v>31.8</v>
+        <v>11</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H98" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I98" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J98" s="3" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
-        <v>11</v>
+        <v>34.648700673724733</v>
       </c>
       <c r="B99" s="2">
-        <v>7</v>
+        <v>25.98652550529355</v>
       </c>
       <c r="C99" s="2">
-        <v>82</v>
+        <v>39.364773820981711</v>
       </c>
       <c r="D99" s="2">
-        <v>82</v>
+        <v>40.9</v>
       </c>
       <c r="E99" s="2">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="F99" s="2">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H99" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I99" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J99" s="3" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
-        <v>34.648700673724733</v>
+        <v>37.278657968313141</v>
       </c>
       <c r="B100" s="2">
-        <v>25.98652550529355</v>
+        <v>44.734389561975775</v>
       </c>
       <c r="C100" s="2">
-        <v>39.364773820981711</v>
+        <v>17.986952469711092</v>
       </c>
       <c r="D100" s="2">
-        <v>40.9</v>
+        <v>19.3</v>
       </c>
       <c r="E100" s="2">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="F100" s="2">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H100" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I100" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J100" s="3" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
-        <v>37.278657968313141</v>
+        <v>31.454918032786889</v>
       </c>
       <c r="B101" s="2">
-        <v>44.734389561975775</v>
+        <v>31.659836065573774</v>
       </c>
       <c r="C101" s="2">
-        <v>17.986952469711092</v>
+        <v>36.885245901639351</v>
       </c>
       <c r="D101" s="2">
-        <v>19.3</v>
+        <v>36</v>
       </c>
       <c r="E101" s="2">
-        <v>48</v>
+        <v>30.9</v>
       </c>
       <c r="F101" s="2">
-        <v>40</v>
+        <v>30.7</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H101" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I101" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J101" s="3" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
-        <v>31.454918032786889</v>
+        <v>36.666666666666671</v>
       </c>
       <c r="B102" s="2">
-        <v>31.659836065573774</v>
+        <v>59.166666666666671</v>
       </c>
       <c r="C102" s="2">
-        <v>36.885245901639351</v>
+        <v>4.166666666666667</v>
       </c>
       <c r="D102" s="2">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="E102" s="2">
-        <v>30.9</v>
+        <v>56.8</v>
       </c>
       <c r="F102" s="2">
-        <v>30.7</v>
+        <v>35.200000000000003</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H102" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I102" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J102" s="3" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
-        <v>36.666666666666671</v>
+        <v>31.609775802868104</v>
       </c>
       <c r="B103" s="2">
-        <v>59.166666666666671</v>
+        <v>65.037366188648747</v>
       </c>
       <c r="C103" s="2">
-        <v>4.166666666666667</v>
+        <v>3.3528580084831341</v>
       </c>
       <c r="D103" s="2">
-        <v>4</v>
+        <v>3.32</v>
       </c>
       <c r="E103" s="2">
-        <v>56.8</v>
+        <v>64.400000000000006</v>
       </c>
       <c r="F103" s="2">
-        <v>35.200000000000003</v>
+        <v>31.3</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H103" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I103" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J103" s="3" t="s">
         <v>56</v>
@@ -3971,191 +3968,191 @@
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
-        <v>31.609775802868104</v>
+        <v>21.643286573146291</v>
       </c>
       <c r="B104" s="2">
-        <v>65.037366188648747</v>
+        <v>11.523046092184368</v>
       </c>
       <c r="C104" s="2">
-        <v>3.3528580084831341</v>
+        <v>66.833667334669329</v>
       </c>
       <c r="D104" s="2">
-        <v>3.32</v>
+        <v>66.7</v>
       </c>
       <c r="E104" s="2">
-        <v>64.400000000000006</v>
+        <v>11.5</v>
       </c>
       <c r="F104" s="2">
-        <v>31.3</v>
+        <v>21.6</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H104" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I104" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J104" s="3" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
-        <v>21.643286573146291</v>
+        <v>31.01807802093245</v>
       </c>
       <c r="B105" s="2">
-        <v>11.523046092184368</v>
+        <v>60.418648905803998</v>
       </c>
       <c r="C105" s="2">
-        <v>66.833667334669329</v>
+        <v>8.5632730732635594</v>
       </c>
       <c r="D105" s="2">
-        <v>66.7</v>
+        <v>9</v>
       </c>
       <c r="E105" s="2">
-        <v>11.5</v>
+        <v>63.5</v>
       </c>
       <c r="F105" s="2">
-        <v>21.6</v>
+        <v>32.6</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H105" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I105" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J105" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
-        <v>31.01807802093245</v>
+        <v>26.886556721639177</v>
       </c>
       <c r="B106" s="2">
-        <v>60.418648905803998</v>
+        <v>66.466766616691658</v>
       </c>
       <c r="C106" s="2">
-        <v>8.5632730732635594</v>
+        <v>6.6466766616691659</v>
       </c>
       <c r="D106" s="2">
-        <v>9</v>
+        <v>6.65</v>
       </c>
       <c r="E106" s="2">
-        <v>63.5</v>
+        <v>66.5</v>
       </c>
       <c r="F106" s="2">
-        <v>32.6</v>
+        <v>26.9</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H106" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I106" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J106" s="3" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
-        <v>26.886556721639177</v>
+        <v>3.5982008995502248</v>
       </c>
       <c r="B107" s="2">
-        <v>66.466766616691658</v>
+        <v>7.4462768615692152</v>
       </c>
       <c r="C107" s="2">
-        <v>6.6466766616691659</v>
+        <v>88.955522238880562</v>
       </c>
       <c r="D107" s="2">
-        <v>6.65</v>
+        <v>89</v>
       </c>
       <c r="E107" s="2">
-        <v>66.5</v>
+        <v>7.45</v>
       </c>
       <c r="F107" s="2">
-        <v>26.9</v>
+        <v>3.6</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H107" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I107" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J107" s="3" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
-        <v>3.5982008995502248</v>
+        <v>32.542579075425792</v>
       </c>
       <c r="B108" s="2">
-        <v>7.4462768615692152</v>
+        <v>65.085158150851584</v>
       </c>
       <c r="C108" s="2">
-        <v>88.955522238880562</v>
+        <v>2.3722627737226274</v>
       </c>
       <c r="D108" s="2">
-        <v>89</v>
+        <v>2.34</v>
       </c>
       <c r="E108" s="2">
-        <v>7.45</v>
+        <v>64.2</v>
       </c>
       <c r="F108" s="2">
-        <v>3.6</v>
+        <v>32.1</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H108" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I108" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J108" s="3" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
-        <v>32.542579075425792</v>
+        <v>33.231675255021564</v>
       </c>
       <c r="B109" s="2">
-        <v>65.085158150851584</v>
+        <v>60.36386581133663</v>
       </c>
       <c r="C109" s="2">
-        <v>2.3722627737226274</v>
+        <v>6.4044589336418127</v>
       </c>
       <c r="D109" s="2">
-        <v>2.34</v>
+        <v>6.09</v>
       </c>
       <c r="E109" s="2">
-        <v>64.2</v>
+        <v>57.4</v>
       </c>
       <c r="F109" s="2">
-        <v>32.1</v>
+        <v>31.6</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H109" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I109" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J109" s="3" t="s">
         <v>56</v>
@@ -4163,377 +4160,377 @@
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
-        <v>33.231675255021564</v>
+        <v>54.154154154154149</v>
       </c>
       <c r="B110" s="2">
-        <v>60.36386581133663</v>
+        <v>32.832832832832828</v>
       </c>
       <c r="C110" s="2">
-        <v>6.4044589336418127</v>
+        <v>13.013013013013012</v>
       </c>
       <c r="D110" s="2">
-        <v>6.09</v>
+        <v>13</v>
       </c>
       <c r="E110" s="2">
-        <v>57.4</v>
+        <v>32.799999999999997</v>
       </c>
       <c r="F110" s="2">
-        <v>31.6</v>
+        <v>54.1</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H110" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I110" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J110" s="3" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
-        <v>54.154154154154149</v>
+        <v>29.399585921325052</v>
       </c>
       <c r="B111" s="2">
-        <v>32.832832832832828</v>
+        <v>46.997929606625256</v>
       </c>
       <c r="C111" s="2">
-        <v>13.013013013013012</v>
+        <v>23.602484472049692</v>
       </c>
       <c r="D111" s="2">
-        <v>13</v>
+        <v>22.8</v>
       </c>
       <c r="E111" s="2">
-        <v>32.799999999999997</v>
+        <v>45.4</v>
       </c>
       <c r="F111" s="2">
-        <v>54.1</v>
+        <v>28.4</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H111" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I111" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J111" s="3" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
-        <v>29.399585921325052</v>
+        <v>3.8540385403854032</v>
       </c>
       <c r="B112" s="2">
-        <v>46.997929606625256</v>
+        <v>2.0500205002050018</v>
       </c>
       <c r="C112" s="2">
-        <v>23.602484472049692</v>
+        <v>94.095940959409575</v>
       </c>
       <c r="D112" s="2">
-        <v>22.8</v>
+        <v>91.8</v>
       </c>
       <c r="E112" s="2">
-        <v>45.4</v>
+        <v>2</v>
       </c>
       <c r="F112" s="2">
-        <v>28.4</v>
+        <v>3.76</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H112" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I112" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J112" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
-        <v>3.8540385403854032</v>
+        <v>8.6629944917376047</v>
       </c>
       <c r="B113" s="2">
-        <v>2.0500205002050018</v>
+        <v>54.28142213319979</v>
       </c>
       <c r="C113" s="2">
-        <v>94.095940959409575</v>
+        <v>37.055583375062589</v>
       </c>
       <c r="D113" s="2">
-        <v>91.8</v>
+        <v>37</v>
       </c>
       <c r="E113" s="2">
-        <v>2</v>
+        <v>54.2</v>
       </c>
       <c r="F113" s="2">
-        <v>3.76</v>
+        <v>8.65</v>
       </c>
       <c r="G113" s="3" t="s">
-        <v>68</v>
+        <v>10</v>
       </c>
       <c r="H113" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I113" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J113" s="3" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
-        <v>27.154308617234474</v>
+        <v>5.5226824457593677</v>
       </c>
       <c r="B114" s="2">
-        <v>45.390781563126254</v>
+        <v>12.721893491124259</v>
       </c>
       <c r="C114" s="2">
-        <v>27.45490981963928</v>
+        <v>81.755424063116365</v>
       </c>
       <c r="D114" s="2">
-        <v>27.4</v>
+        <v>82.9</v>
       </c>
       <c r="E114" s="2">
-        <v>45.3</v>
+        <v>12.9</v>
       </c>
       <c r="F114" s="2">
-        <v>27.1</v>
+        <v>5.6</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="H114" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I114" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J114" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
-        <v>8.6629944917376047</v>
+        <v>4.2095790420957906</v>
       </c>
       <c r="B115" s="2">
-        <v>54.28142213319979</v>
+        <v>17.498250174982502</v>
       </c>
       <c r="C115" s="2">
-        <v>37.055583375062589</v>
+        <v>78.292170782921715</v>
       </c>
       <c r="D115" s="2">
-        <v>37</v>
+        <v>78.3</v>
       </c>
       <c r="E115" s="2">
-        <v>54.2</v>
+        <v>17.5</v>
       </c>
       <c r="F115" s="2">
-        <v>8.65</v>
+        <v>4.21</v>
       </c>
       <c r="G115" s="3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H115" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I115" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J115" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
-        <v>5.5226824457593677</v>
+        <v>11.84738955823293</v>
       </c>
       <c r="B116" s="2">
-        <v>12.721893491124259</v>
+        <v>33.232931726907623</v>
       </c>
       <c r="C116" s="2">
-        <v>81.755424063116365</v>
+        <v>54.91967871485943</v>
       </c>
       <c r="D116" s="2">
-        <v>82.9</v>
+        <v>54.7</v>
       </c>
       <c r="E116" s="2">
-        <v>12.9</v>
+        <v>33.1</v>
       </c>
       <c r="F116" s="2">
-        <v>5.6</v>
+        <v>11.8</v>
       </c>
       <c r="G116" s="3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="H116" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I116" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J116" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
-        <v>4.2095790420957906</v>
+        <v>16.701030927835049</v>
       </c>
       <c r="B117" s="2">
-        <v>17.498250174982502</v>
+        <v>31.649484536082468</v>
       </c>
       <c r="C117" s="2">
-        <v>78.292170782921715</v>
+        <v>51.649484536082468</v>
       </c>
       <c r="D117" s="2">
-        <v>78.3</v>
+        <v>50.1</v>
       </c>
       <c r="E117" s="2">
-        <v>17.5</v>
+        <v>30.7</v>
       </c>
       <c r="F117" s="2">
-        <v>4.21</v>
+        <v>16.2</v>
       </c>
       <c r="G117" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H117" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I117" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J117" s="3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
-        <v>11.84738955823293</v>
+        <v>48.68292682926829</v>
       </c>
       <c r="B118" s="2">
-        <v>33.232931726907623</v>
+        <v>32.195121951219512</v>
       </c>
       <c r="C118" s="2">
-        <v>54.91967871485943</v>
+        <v>19.121951219512194</v>
       </c>
       <c r="D118" s="2">
-        <v>54.7</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="E118" s="2">
-        <v>33.1</v>
+        <v>33</v>
       </c>
       <c r="F118" s="2">
-        <v>11.8</v>
+        <v>49.9</v>
       </c>
       <c r="G118" s="3" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="H118" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I118" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J118" s="3" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
-        <v>16.701030927835049</v>
+        <v>31.573604060913706</v>
       </c>
       <c r="B119" s="2">
-        <v>31.649484536082468</v>
+        <v>18.071065989847714</v>
       </c>
       <c r="C119" s="2">
-        <v>51.649484536082468</v>
+        <v>50.35532994923858</v>
       </c>
       <c r="D119" s="2">
-        <v>50.1</v>
+        <v>49.6</v>
       </c>
       <c r="E119" s="2">
-        <v>30.7</v>
+        <v>17.8</v>
       </c>
       <c r="F119" s="2">
-        <v>16.2</v>
+        <v>31.1</v>
       </c>
       <c r="G119" s="3" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="H119" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I119" s="3" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="J119" s="3" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
-        <v>48.68292682926829</v>
+        <v>31.362725450901809</v>
       </c>
       <c r="B120" s="2">
-        <v>32.195121951219512</v>
+        <v>18.537074148296597</v>
       </c>
       <c r="C120" s="2">
-        <v>19.121951219512194</v>
+        <v>50.100200400801612</v>
       </c>
       <c r="D120" s="2">
-        <v>19.600000000000001</v>
+        <v>50</v>
       </c>
       <c r="E120" s="2">
-        <v>33</v>
+        <v>18.5</v>
       </c>
       <c r="F120" s="2">
-        <v>49.9</v>
+        <v>31.3</v>
       </c>
       <c r="G120" s="3" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="H120" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I120" s="3" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="J120" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
-        <v>31.573604060913706</v>
+        <v>45.273631840796021</v>
       </c>
       <c r="B121" s="2">
-        <v>18.071065989847714</v>
+        <v>21.890547263681594</v>
       </c>
       <c r="C121" s="2">
-        <v>50.35532994923858</v>
+        <v>32.835820895522389</v>
       </c>
       <c r="D121" s="2">
-        <v>49.6</v>
+        <v>33</v>
       </c>
       <c r="E121" s="2">
-        <v>17.8</v>
+        <v>22</v>
       </c>
       <c r="F121" s="2">
-        <v>31.1</v>
+        <v>45.5</v>
       </c>
       <c r="G121" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H121" s="3" t="s">
         <v>11</v>
@@ -4542,70 +4539,6 @@
         <v>12</v>
       </c>
       <c r="J121" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A122" s="2">
-        <v>31.362725450901809</v>
-      </c>
-      <c r="B122" s="2">
-        <v>18.537074148296597</v>
-      </c>
-      <c r="C122" s="2">
-        <v>50.100200400801612</v>
-      </c>
-      <c r="D122" s="2">
-        <v>50</v>
-      </c>
-      <c r="E122" s="2">
-        <v>18.5</v>
-      </c>
-      <c r="F122" s="2">
-        <v>31.3</v>
-      </c>
-      <c r="G122" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="H122" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I122" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J122" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A123" s="2">
-        <v>45.273631840796021</v>
-      </c>
-      <c r="B123" s="2">
-        <v>21.890547263681594</v>
-      </c>
-      <c r="C123" s="2">
-        <v>32.835820895522389</v>
-      </c>
-      <c r="D123" s="2">
-        <v>33</v>
-      </c>
-      <c r="E123" s="2">
-        <v>22</v>
-      </c>
-      <c r="F123" s="2">
-        <v>45.5</v>
-      </c>
-      <c r="G123" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="H123" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I123" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J123" s="3" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>